<commit_message>
update actives page and EC
</commit_message>
<xml_diff>
--- a/images/Headshots/Update Headshots/HeadshotList.xlsx
+++ b/images/Headshots/Update Headshots/HeadshotList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshernandez/Desktop/ben0815.github.io/images/Headshots/Update Headshots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\ben0815.github.io\images\Headshots\Update Headshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C618402-9A0C-5644-A766-C8CBF645F60F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C7050E-29BB-47ED-A212-EF19D56E9617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19220" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="124">
   <si>
     <t>Full Name</t>
   </si>
@@ -142,12 +142,6 @@
   </si>
   <si>
     <t>tony.jpg</t>
-  </si>
-  <si>
-    <t>Mary Visconti</t>
-  </si>
-  <si>
-    <t>mary.jpg</t>
   </si>
   <si>
     <t>Cecile Savoie</t>
@@ -811,22 +805,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625"/>
-    <col min="2" max="2" width="13.1640625"/>
-    <col min="3" max="5" width="8.5"/>
-    <col min="6" max="6" width="14.83203125"/>
-    <col min="7" max="1025" width="8.5"/>
+    <col min="1" max="1" width="17.109375"/>
+    <col min="2" max="2" width="13.109375"/>
+    <col min="3" max="5" width="8.44140625"/>
+    <col min="6" max="6" width="14.77734375"/>
+    <col min="7" max="7" width="8.44140625"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -849,31 +845,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -884,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -895,29 +889,23 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -928,14 +916,14 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -946,14 +934,14 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -963,66 +951,66 @@
       <c r="C10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1033,8 +1021,14 @@
         <f>FALSE()</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1046,19 +1040,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>46</v>
       </c>
       <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1070,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1082,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1094,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1106,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1118,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1126,22 +1119,22 @@
         <v>59</v>
       </c>
       <c r="C22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
       <c r="B23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C23" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -1153,7 +1146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -1165,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -1177,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -1189,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -1201,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -1213,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1225,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -1237,294 +1230,281 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C32" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>100</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B49" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B54" t="s">
         <v>121</v>
       </c>
-      <c r="C40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" t="s">
-        <v>125</v>
-      </c>
-      <c r="C41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C43" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B46" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" t="s">
-        <v>119</v>
-      </c>
       <c r="C54" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B55" t="s">
-        <v>123</v>
-      </c>
-      <c r="C55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
update rush flyer and actives page
</commit_message>
<xml_diff>
--- a/images/Headshots/Update Headshots/HeadshotList.xlsx
+++ b/images/Headshots/Update Headshots/HeadshotList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\ben0815.github.io\images\Headshots\Update Headshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C7050E-29BB-47ED-A212-EF19D56E9617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A033E40-EE95-497A-BD5C-1027ACD7CCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="3684" windowWidth="30960" windowHeight="12120" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>Full Name</t>
   </si>
@@ -45,12 +45,6 @@
     <t>On EC?</t>
   </si>
   <si>
-    <t>Grace Andersen</t>
-  </si>
-  <si>
-    <t>grace.jpg</t>
-  </si>
-  <si>
     <t>Austin Peterson</t>
   </si>
   <si>
@@ -69,9 +63,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Marshall</t>
-  </si>
-  <si>
     <t>Caleb Alpire</t>
   </si>
   <si>
@@ -81,15 +72,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>Regent</t>
-  </si>
-  <si>
-    <t>Jamaal Roberson</t>
-  </si>
-  <si>
-    <t>jamaal.jpg</t>
-  </si>
-  <si>
     <t>VR</t>
   </si>
   <si>
@@ -102,42 +84,18 @@
     <t>Treasurer</t>
   </si>
   <si>
-    <t>David turlip</t>
-  </si>
-  <si>
-    <t>david.jpg</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
     <t>Scribe</t>
   </si>
   <si>
-    <t>Kelsie Alexander</t>
-  </si>
-  <si>
-    <t>kelsie.jpg</t>
-  </si>
-  <si>
     <t>CS</t>
   </si>
   <si>
-    <t>Corsec</t>
-  </si>
-  <si>
-    <t>Jackson Wicker</t>
-  </si>
-  <si>
-    <t>jackson.jpg</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
-    <t>Pledge Marshall</t>
-  </si>
-  <si>
     <t>Anthony Mele</t>
   </si>
   <si>
@@ -156,18 +114,6 @@
     <t>jake.jpg</t>
   </si>
   <si>
-    <t>Sohan Rahman</t>
-  </si>
-  <si>
-    <t>sohan.jpg</t>
-  </si>
-  <si>
-    <t>Yonathan Zetune</t>
-  </si>
-  <si>
-    <t>yonathan.jpg</t>
-  </si>
-  <si>
     <t>Oscar Martinez</t>
   </si>
   <si>
@@ -180,12 +126,6 @@
     <t>gavin.jpg</t>
   </si>
   <si>
-    <t>Remi Emmot</t>
-  </si>
-  <si>
-    <t>remi.jpg</t>
-  </si>
-  <si>
     <t>Alexa Milstein</t>
   </si>
   <si>
@@ -204,18 +144,6 @@
     <t>hillaire.jpg</t>
   </si>
   <si>
-    <t>Sumedh Khair</t>
-  </si>
-  <si>
-    <t>sumedh.jpg</t>
-  </si>
-  <si>
-    <t>Jackson Bartay</t>
-  </si>
-  <si>
-    <t>jacksonB.jpg</t>
-  </si>
-  <si>
     <t>Neida Cruz</t>
   </si>
   <si>
@@ -234,18 +162,6 @@
     <t>christian.jpg</t>
   </si>
   <si>
-    <t>Felix Kainz</t>
-  </si>
-  <si>
-    <t>felix.jpg</t>
-  </si>
-  <si>
-    <t>Marissa Peters</t>
-  </si>
-  <si>
-    <t>marissa.jpg</t>
-  </si>
-  <si>
     <t>Jake Spooner</t>
   </si>
   <si>
@@ -279,9 +195,6 @@
     <t>Sydney Montoya</t>
   </si>
   <si>
-    <t>Sarah Neidhardt</t>
-  </si>
-  <si>
     <t>Samuel Behrens</t>
   </si>
   <si>
@@ -342,9 +255,6 @@
     <t>max.jpg</t>
   </si>
   <si>
-    <t>sarahn.jpg</t>
-  </si>
-  <si>
     <t>sam.jpg</t>
   </si>
   <si>
@@ -402,10 +312,16 @@
     <t>julian.jpg</t>
   </si>
   <si>
-    <t>Autumn Cook</t>
-  </si>
-  <si>
-    <t>autumn.jpg</t>
+    <t>Hannah Lilly</t>
+  </si>
+  <si>
+    <t>hannah.jpg</t>
+  </si>
+  <si>
+    <t>Ben Griffin</t>
+  </si>
+  <si>
+    <t>ben.jpg</t>
   </si>
 </sst>
 </file>
@@ -805,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,53 +757,61 @@
         <v>4</v>
       </c>
       <c r="C2" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
+      <c r="G5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -897,143 +821,110 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="5"/>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" t="b">
         <f>FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="C11" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C13" t="b">
         <f>FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C14" t="b">
         <f>FALSE()</f>
         <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15" t="b">
         <f>FALSE()</f>
@@ -1042,21 +933,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="C16" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C17" t="b">
         <f>FALSE()</f>
@@ -1065,10 +957,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C18" t="b">
         <f>FALSE()</f>
@@ -1077,10 +969,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C19" t="b">
         <f>FALSE()</f>
@@ -1089,141 +981,136 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C21" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>76</v>
-      </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C31" t="b">
         <f>FALSE()</f>
@@ -1232,21 +1119,22 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C32" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C33" t="b">
         <f>FALSE()</f>
@@ -1255,21 +1143,22 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" t="s">
-        <v>18</v>
+        <v>81</v>
+      </c>
+      <c r="C34" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C35" t="b">
         <f>FALSE()</f>
@@ -1278,21 +1167,22 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" t="s">
-        <v>20</v>
+        <v>83</v>
+      </c>
+      <c r="C36" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="C37" t="b">
         <f>FALSE()</f>
@@ -1301,10 +1191,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C38" t="b">
         <f>FALSE()</f>
@@ -1313,198 +1203,56 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="C39" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>122</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="C40" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C41" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C43" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C45" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B46" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C48" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C50" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B52" t="s">
-        <v>116</v>
-      </c>
-      <c r="C52" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B54" t="s">
-        <v>121</v>
-      </c>
-      <c r="C54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
+      <c r="C42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
update headshots - fall2021 pledge class
also light photo cleanup
</commit_message>
<xml_diff>
--- a/images/Headshots/Update Headshots/HeadshotList.xlsx
+++ b/images/Headshots/Update Headshots/HeadshotList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\ben0815.github.io\images\Headshots\Update Headshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A033E40-EE95-497A-BD5C-1027ACD7CCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B56A615-BFF7-4682-814F-AE95BE85EA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="3684" windowWidth="30960" windowHeight="12120" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
   <si>
     <t>Full Name</t>
   </si>
@@ -322,6 +322,147 @@
   </si>
   <si>
     <t>ben.jpg</t>
+  </si>
+  <si>
+    <t>Tanner Waters</t>
+  </si>
+  <si>
+    <t>Aiden Long</t>
+  </si>
+  <si>
+    <t>Dario Emad</t>
+  </si>
+  <si>
+    <t>Blake Hajdik</t>
+  </si>
+  <si>
+    <t>Avantika Chellury</t>
+  </si>
+  <si>
+    <t>Christian Falk</t>
+  </si>
+  <si>
+    <t>Kat Eller</t>
+  </si>
+  <si>
+    <t>Megan Barry</t>
+  </si>
+  <si>
+    <t>Aiden Mitchell</t>
+  </si>
+  <si>
+    <t>Priscila Santos</t>
+  </si>
+  <si>
+    <t>Duncan Brown</t>
+  </si>
+  <si>
+    <t>Mikayla Wiest</t>
+  </si>
+  <si>
+    <t>Emma Rader</t>
+  </si>
+  <si>
+    <t>Connor Malone</t>
+  </si>
+  <si>
+    <t>Adam Vick</t>
+  </si>
+  <si>
+    <t>Aayushi Saxena</t>
+  </si>
+  <si>
+    <t>Shaunak Dabir</t>
+  </si>
+  <si>
+    <t>Juan Peña</t>
+  </si>
+  <si>
+    <t>Troy Davis</t>
+  </si>
+  <si>
+    <t>Rosendo Torres</t>
+  </si>
+  <si>
+    <t>Abhi Bhattacharyya</t>
+  </si>
+  <si>
+    <t>Ryan Crowell</t>
+  </si>
+  <si>
+    <t>Avery Austin</t>
+  </si>
+  <si>
+    <t>Cristina Austgen</t>
+  </si>
+  <si>
+    <t>Olivia Huhn</t>
+  </si>
+  <si>
+    <t>Qynton De Los Santos</t>
+  </si>
+  <si>
+    <t>Camryn Wagner</t>
+  </si>
+  <si>
+    <t>Tristan Koster</t>
+  </si>
+  <si>
+    <t>Aidan Rader</t>
+  </si>
+  <si>
+    <t>Will Davis</t>
+  </si>
+  <si>
+    <t>Weston Browning</t>
+  </si>
+  <si>
+    <t>Chris Mendez</t>
+  </si>
+  <si>
+    <t>rosendo.JPG</t>
+  </si>
+  <si>
+    <t>abhi.JPG</t>
+  </si>
+  <si>
+    <t>ryan.JPG</t>
+  </si>
+  <si>
+    <t>cristina.JPG</t>
+  </si>
+  <si>
+    <t>olivia.JPG</t>
+  </si>
+  <si>
+    <t>qynton.JPG</t>
+  </si>
+  <si>
+    <t>tristan.JPG</t>
+  </si>
+  <si>
+    <t>weston.JPG</t>
+  </si>
+  <si>
+    <t>averyA.JPG</t>
+  </si>
+  <si>
+    <t>cami.JPG</t>
+  </si>
+  <si>
+    <t>aiden.JPG</t>
+  </si>
+  <si>
+    <t>willJ.JPG</t>
+  </si>
+  <si>
+    <t>chrisM.JPG</t>
+  </si>
+  <si>
+    <t>Sharleen Faruque</t>
+  </si>
+  <si>
+    <t>sharleen.jpg</t>
   </si>
 </sst>
 </file>
@@ -400,13 +541,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,79 +958,78 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
+        <v>142</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" t="b">
+        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="b">
-        <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="b">
         <f>FALSE()</f>
@@ -897,10 +1038,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="b">
         <f>FALSE()</f>
@@ -909,10 +1050,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="b">
         <f>FALSE()</f>
@@ -921,10 +1062,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="b">
         <f>FALSE()</f>
@@ -933,322 +1074,531 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C16" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C17" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="C17" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="C18" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C19" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="C20" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>49</v>
       </c>
-      <c r="C20" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="C21" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="C22" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="C23" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="P24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="P25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="C26" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="P27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="C27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>75</v>
       </c>
-      <c r="C28" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="C29" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>76</v>
       </c>
-      <c r="C29" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="C30" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>77</v>
       </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>78</v>
       </c>
-      <c r="C31" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="C32" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="C32" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="C33" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>80</v>
       </c>
-      <c r="C33" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="C34" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c r="C34" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="C35" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>82</v>
       </c>
-      <c r="C35" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="C36" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>83</v>
       </c>
-      <c r="C36" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="C37" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>84</v>
       </c>
-      <c r="C37" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="C38" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>85</v>
       </c>
-      <c r="C38" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="C39" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>86</v>
       </c>
-      <c r="C39" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="C40" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>87</v>
       </c>
-      <c r="C40" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="C41" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>91</v>
       </c>
-      <c r="C41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>93</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added emma R headshot
</commit_message>
<xml_diff>
--- a/images/Headshots/Update Headshots/HeadshotList.xlsx
+++ b/images/Headshots/Update Headshots/HeadshotList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\ben0815.github.io\images\Headshots\Update Headshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B56A615-BFF7-4682-814F-AE95BE85EA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D508C-283F-46BE-84B4-7298C778D9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="144">
   <si>
     <t>Full Name</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>sharleen.jpg</t>
+  </si>
+  <si>
+    <t>emmaR.jpg</t>
   </si>
 </sst>
 </file>
@@ -863,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1458,11 +1461,11 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>115</v>
+      <c r="A44" t="s">
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -1470,10 +1473,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -1481,10 +1484,10 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -1492,10 +1495,10 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -1503,10 +1506,10 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -1514,10 +1517,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -1525,10 +1528,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -1536,10 +1539,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -1547,10 +1550,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -1558,10 +1561,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -1569,10 +1572,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -1580,10 +1583,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -1591,12 +1594,23 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>140</v>
       </c>
-      <c r="C56" t="b">
+      <c r="C57" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated EC for this semester & fixed a typo
</commit_message>
<xml_diff>
--- a/images/Headshots/Update Headshots/HeadshotList.xlsx
+++ b/images/Headshots/Update Headshots/HeadshotList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Documents\ben0815.github.io\images\Headshots\Update Headshots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohuhn\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB46E06-781D-49BB-8346-0DFB307E0117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A49215-CEA8-49F5-A2C3-AB6E124BC9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8964" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,8 +922,8 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -944,13 +944,13 @@
       <c r="B5" t="s">
         <v>95</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -987,8 +987,8 @@
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
+      <c r="C8" t="b">
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -1210,8 +1210,8 @@
       <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
-        <v>8</v>
+      <c r="C25" t="b">
+        <v>0</v>
       </c>
       <c r="P25" t="s">
         <v>100</v>
@@ -1239,8 +1239,8 @@
       <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
-        <v>16</v>
+      <c r="C27" t="b">
+        <v>0</v>
       </c>
       <c r="P27" t="s">
         <v>102</v>
@@ -1311,9 +1311,8 @@
       <c r="B32" t="s">
         <v>78</v>
       </c>
-      <c r="C32" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+      <c r="C32" t="s">
+        <v>8</v>
       </c>
       <c r="P32" t="s">
         <v>107</v>
@@ -1504,7 +1503,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>144</v>
       </c>
       <c r="B47" t="s">
@@ -1554,8 +1553,8 @@
       <c r="B51" t="s">
         <v>131</v>
       </c>
-      <c r="C51" t="b">
-        <v>0</v>
+      <c r="C51" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1609,8 +1608,8 @@
       <c r="B56" t="s">
         <v>138</v>
       </c>
-      <c r="C56" t="b">
-        <v>0</v>
+      <c r="C56" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>